<commit_message>
Exp group edits for EK
</commit_message>
<xml_diff>
--- a/data/pokemon.xlsx
+++ b/data/pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\EKhelper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C252E4F-C392-496F-8F03-5C3A3DF28BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2542A0A6-274F-4DA9-BB6F-2D40E4E2F28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4780,6 +4780,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="212" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="203" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4834,9 +4837,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="212" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5174,8 +5174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A363" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L379" sqref="L379"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5193,18 +5193,18 @@
       <c r="B1" s="208" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="210" t="s">
+      <c r="C1" s="211" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="211"/>
-      <c r="E1" s="211"/>
-      <c r="F1" s="211"/>
-      <c r="G1" s="211"/>
-      <c r="H1" s="211"/>
-      <c r="I1" s="222" t="s">
+      <c r="D1" s="212"/>
+      <c r="E1" s="212"/>
+      <c r="F1" s="212"/>
+      <c r="G1" s="212"/>
+      <c r="H1" s="212"/>
+      <c r="I1" s="223" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="223"/>
+      <c r="J1" s="224"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5231,8 +5231,8 @@
       <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="224"/>
-      <c r="J2" s="225"/>
+      <c r="I2" s="225"/>
+      <c r="J2" s="226"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -5679,13 +5679,13 @@
         <v>65</v>
       </c>
       <c r="D17">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E17">
         <v>40</v>
       </c>
       <c r="F17">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G17">
         <v>80</v>
@@ -6107,22 +6107,22 @@
       <c r="B31" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="238">
+      <c r="C31" s="210">
         <v>55</v>
       </c>
-      <c r="D31" s="238">
+      <c r="D31" s="210">
         <v>47</v>
       </c>
-      <c r="E31" s="238">
+      <c r="E31" s="210">
         <v>52</v>
       </c>
-      <c r="F31" s="238">
+      <c r="F31" s="210">
         <v>40</v>
       </c>
-      <c r="G31" s="238">
+      <c r="G31" s="210">
         <v>40</v>
       </c>
-      <c r="H31" s="238">
+      <c r="H31" s="210">
         <v>41</v>
       </c>
       <c r="I31" s="61" t="s">
@@ -6199,22 +6199,22 @@
       <c r="B34" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="238">
+      <c r="C34" s="210">
         <v>46</v>
       </c>
-      <c r="D34" s="238">
+      <c r="D34" s="210">
         <v>57</v>
       </c>
-      <c r="E34" s="238">
+      <c r="E34" s="210">
         <v>40</v>
       </c>
-      <c r="F34" s="238">
+      <c r="F34" s="210">
         <v>40</v>
       </c>
-      <c r="G34" s="238">
+      <c r="G34" s="210">
         <v>40</v>
       </c>
-      <c r="H34" s="238">
+      <c r="H34" s="210">
         <v>50</v>
       </c>
       <c r="I34" s="65" t="s">
@@ -16377,10 +16377,10 @@
       <c r="H363">
         <v>85</v>
       </c>
-      <c r="I363" s="232" t="s">
+      <c r="I363" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="J363" s="233"/>
+      <c r="J363" s="234"/>
     </row>
     <row r="364" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A364" s="2">
@@ -16407,10 +16407,10 @@
       <c r="H364">
         <v>85</v>
       </c>
-      <c r="I364" s="234" t="s">
+      <c r="I364" s="235" t="s">
         <v>27</v>
       </c>
-      <c r="J364" s="235"/>
+      <c r="J364" s="236"/>
     </row>
     <row r="365" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A365" s="2">
@@ -16565,10 +16565,10 @@
       <c r="H369">
         <v>40</v>
       </c>
-      <c r="I369" s="228" t="s">
+      <c r="I369" s="229" t="s">
         <v>85</v>
       </c>
-      <c r="J369" s="229"/>
+      <c r="J369" s="230"/>
     </row>
     <row r="370" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A370" s="2">
@@ -16595,10 +16595,10 @@
       <c r="H370">
         <v>50</v>
       </c>
-      <c r="I370" s="228" t="s">
+      <c r="I370" s="229" t="s">
         <v>85</v>
       </c>
-      <c r="J370" s="229"/>
+      <c r="J370" s="230"/>
     </row>
     <row r="371" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A371" s="2">
@@ -16625,10 +16625,10 @@
       <c r="H371">
         <v>90</v>
       </c>
-      <c r="I371" s="230" t="s">
+      <c r="I371" s="231" t="s">
         <v>85</v>
       </c>
-      <c r="J371" s="231"/>
+      <c r="J371" s="232"/>
     </row>
     <row r="372" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A372" s="2">
@@ -16655,10 +16655,10 @@
       <c r="H372">
         <v>50</v>
       </c>
-      <c r="I372" s="226" t="s">
+      <c r="I372" s="227" t="s">
         <v>174</v>
       </c>
-      <c r="J372" s="227"/>
+      <c r="J372" s="228"/>
     </row>
     <row r="373" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A373" s="2">
@@ -16685,10 +16685,10 @@
       <c r="H373">
         <v>50</v>
       </c>
-      <c r="I373" s="226" t="s">
+      <c r="I373" s="227" t="s">
         <v>174</v>
       </c>
-      <c r="J373" s="227"/>
+      <c r="J373" s="228"/>
     </row>
     <row r="374" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A374" s="2">
@@ -16843,10 +16843,10 @@
       <c r="H378">
         <v>50</v>
       </c>
-      <c r="I378" s="214" t="s">
+      <c r="I378" s="215" t="s">
         <v>97</v>
       </c>
-      <c r="J378" s="215"/>
+      <c r="J378" s="216"/>
     </row>
     <row r="379" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A379" s="2">
@@ -16873,10 +16873,10 @@
       <c r="H379">
         <v>50</v>
       </c>
-      <c r="I379" s="216" t="s">
+      <c r="I379" s="217" t="s">
         <v>112</v>
       </c>
-      <c r="J379" s="217"/>
+      <c r="J379" s="218"/>
     </row>
     <row r="380" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A380" s="2">
@@ -16903,10 +16903,10 @@
       <c r="H380">
         <v>50</v>
       </c>
-      <c r="I380" s="218" t="s">
+      <c r="I380" s="219" t="s">
         <v>105</v>
       </c>
-      <c r="J380" s="219"/>
+      <c r="J380" s="220"/>
     </row>
     <row r="381" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A381" s="2">
@@ -16933,10 +16933,10 @@
       <c r="H381">
         <v>90</v>
       </c>
-      <c r="I381" s="220" t="s">
+      <c r="I381" s="221" t="s">
         <v>23</v>
       </c>
-      <c r="J381" s="221"/>
+      <c r="J381" s="222"/>
     </row>
     <row r="382" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A382" s="2">
@@ -16963,10 +16963,10 @@
       <c r="H382">
         <v>90</v>
       </c>
-      <c r="I382" s="236" t="s">
+      <c r="I382" s="237" t="s">
         <v>47</v>
       </c>
-      <c r="J382" s="237"/>
+      <c r="J382" s="238"/>
     </row>
     <row r="383" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A383" s="2">
@@ -17121,10 +17121,10 @@
       <c r="H387">
         <v>150</v>
       </c>
-      <c r="I387" s="228" t="s">
+      <c r="I387" s="229" t="s">
         <v>85</v>
       </c>
-      <c r="J387" s="229"/>
+      <c r="J387" s="230"/>
     </row>
     <row r="388" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A388" s="36">
@@ -17151,10 +17151,10 @@
       <c r="H388">
         <v>65</v>
       </c>
-      <c r="I388" s="212" t="s">
+      <c r="I388" s="213" t="s">
         <v>85</v>
       </c>
-      <c r="J388" s="213"/>
+      <c r="J388" s="214"/>
     </row>
     <row r="389" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>